<commit_message>
fix: support upto 15 skills per role
</commit_message>
<xml_diff>
--- a/src/template.xlsx
+++ b/src/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ben\projects\Planning-Inspectorate\ddat-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ben\projects\Planning-Inspectorate\ddat-templates\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A197D5D4-B544-4598-9E86-2E0420C6A451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1C326B-3345-412D-84C1-25457B0B817D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Self-Assessment" sheetId="1" r:id="rId1"/>
@@ -1927,10 +1927,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2260,7 +2260,7 @@
       <c r="F22" s="153"/>
       <c r="G22" s="29"/>
       <c r="H22" s="178"/>
-      <c r="I22" s="30"/>
+      <c r="I22" s="178"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -2272,7 +2272,7 @@
       <c r="F23" s="153"/>
       <c r="G23" s="29"/>
       <c r="H23" s="178"/>
-      <c r="I23" s="30"/>
+      <c r="I23" s="178"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -2304,24 +2304,84 @@
       <c r="B26" s="25"/>
       <c r="C26" s="26"/>
       <c r="D26" s="27"/>
-      <c r="E26" s="176"/>
+      <c r="E26" s="28"/>
       <c r="F26" s="153"/>
       <c r="G26" s="29"/>
       <c r="H26" s="178"/>
-      <c r="I26" s="30"/>
+      <c r="I26" s="178"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="31"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="34"/>
+    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="153"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="178"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="24"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="153"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="178"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="24"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="153"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="178"/>
+      <c r="I29" s="178"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="24"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="153"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="178"/>
+      <c r="I30" s="178"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="24"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="176"/>
+      <c r="F31" s="153"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="178"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="31"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2348,7 +2408,7 @@
           <x14:formula1>
             <xm:f>'Data Validation'!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G17:G26</xm:sqref>
+          <xm:sqref>G17:G31</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2362,10 +2422,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2925,7 +2985,7 @@
       <c r="O18" s="30"/>
       <c r="P18" s="41"/>
     </row>
-    <row r="19" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="162" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="25">
         <f>('Self-Assessment'!B22)</f>
@@ -2960,20 +3020,14 @@
         <f>('Self-Assessment'!I22)</f>
         <v>0</v>
       </c>
-      <c r="K19" s="63"/>
+      <c r="K19" s="41"/>
       <c r="L19" s="30"/>
-      <c r="M19" s="29" t="str">
-        <f>IFERROR(VLOOKUP(L19,'Data Validation'!$B$2:$C$4,2)," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N19" s="29" t="str" cm="1">
-        <f t="array" ref="N19">IFERROR(_xlfn.IFS($H19-$M19=2,'Data Validation'!$D$2,$H19-$M19=1,'Data Validation'!$D$3,$H19-$M19=0,'Data Validation'!$D$4,$H19-$M19=-1,'Data Validation'!$D$5,$H19-$M19=-2,'Data Validation'!$D$6)," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
       <c r="O19" s="30"/>
-      <c r="P19" s="63"/>
-    </row>
-    <row r="20" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P19" s="41"/>
+    </row>
+    <row r="20" spans="1:16" ht="162" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="61"/>
       <c r="B20" s="25">
         <f>('Self-Assessment'!B23)</f>
@@ -3010,18 +3064,12 @@
       </c>
       <c r="K20" s="41"/>
       <c r="L20" s="30"/>
-      <c r="M20" s="29" t="str">
-        <f>IFERROR(VLOOKUP(L20,'Data Validation'!$B$2:$C$4,2)," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N20" s="29" t="str" cm="1">
-        <f t="array" ref="N20">IFERROR(_xlfn.IFS($H20-$M20=2,'Data Validation'!$D$2,$H20-$M20=1,'Data Validation'!$D$3,$H20-$M20=0,'Data Validation'!$D$4,$H20-$M20=-1,'Data Validation'!$D$5,$H20-$M20=-2,'Data Validation'!$D$6)," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
       <c r="O20" s="30"/>
-      <c r="P20" s="63"/>
-    </row>
-    <row r="21" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P20" s="41"/>
+    </row>
+    <row r="21" spans="1:16" ht="162" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="61"/>
       <c r="B21" s="25">
         <f>('Self-Assessment'!B24)</f>
@@ -3058,18 +3106,12 @@
       </c>
       <c r="K21" s="41"/>
       <c r="L21" s="30"/>
-      <c r="M21" s="29" t="str">
-        <f>IFERROR(VLOOKUP(L21,'Data Validation'!$B$2:$C$4,2)," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N21" s="29" t="str" cm="1">
-        <f t="array" ref="N21">IFERROR(_xlfn.IFS($H21-$M21=2,'Data Validation'!$D$2,$H21-$M21=1,'Data Validation'!$D$3,$H21-$M21=0,'Data Validation'!$D$4,$H21-$M21=-1,'Data Validation'!$D$5,$H21-$M21=-2,'Data Validation'!$D$6)," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
       <c r="O21" s="30"/>
-      <c r="P21" s="63"/>
-    </row>
-    <row r="22" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P21" s="41"/>
+    </row>
+    <row r="22" spans="1:16" ht="162" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="61"/>
       <c r="B22" s="25">
         <f>('Self-Assessment'!B25)</f>
@@ -3106,18 +3148,12 @@
       </c>
       <c r="K22" s="41"/>
       <c r="L22" s="30"/>
-      <c r="M22" s="29" t="str">
-        <f>IFERROR(VLOOKUP(L22,'Data Validation'!$B$2:$C$4,2)," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N22" s="29" t="str" cm="1">
-        <f t="array" ref="N22">IFERROR(_xlfn.IFS($H22-$M22=2,'Data Validation'!$D$2,$H22-$M22=1,'Data Validation'!$D$3,$H22-$M22=0,'Data Validation'!$D$4,$H22-$M22=-1,'Data Validation'!$D$5,$H22-$M22=-2,'Data Validation'!$D$6)," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
       <c r="O22" s="30"/>
-      <c r="P22" s="63"/>
-    </row>
-    <row r="23" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P22" s="41"/>
+    </row>
+    <row r="23" spans="1:16" ht="162" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="61"/>
       <c r="B23" s="25">
         <f>('Self-Assessment'!B26)</f>
@@ -3154,355 +3190,589 @@
       </c>
       <c r="K23" s="41"/>
       <c r="L23" s="30"/>
-      <c r="M23" s="29" t="str">
-        <f>IFERROR(VLOOKUP(L23,'Data Validation'!$B$2:$C$4,2)," ")</f>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="41"/>
+    </row>
+    <row r="24" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="61"/>
+      <c r="B24" s="25">
+        <f>('Self-Assessment'!B27)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="26">
+        <f>('Self-Assessment'!C27)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="27">
+        <f>('Self-Assessment'!D27)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="28">
+        <f>('Self-Assessment'!E27)</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="159"/>
+      <c r="G24" s="62">
+        <f>('Self-Assessment'!G27)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="62" t="str">
+        <f>IFERROR(VLOOKUP(G24,'Data Validation'!$B$2:$C$4,2)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="N23" s="29" t="str" cm="1">
-        <f t="array" ref="N23">IFERROR(_xlfn.IFS($H23-$M23=2,'Data Validation'!$D$2,$H23-$M23=1,'Data Validation'!$D$3,$H23-$M23=0,'Data Validation'!$D$4,$H23-$M23=-1,'Data Validation'!$D$5,$H23-$M23=-2,'Data Validation'!$D$6)," ")</f>
+      <c r="I24" s="62">
+        <f>('Self-Assessment'!H27)</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="62">
+        <f>('Self-Assessment'!I27)</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="63"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="29" t="str">
+        <f>IFERROR(VLOOKUP(L24,'Data Validation'!$B$2:$C$4,2)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O23" s="30"/>
-      <c r="P23" s="63"/>
-    </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="36"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="63"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="65"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="47"/>
+      <c r="N24" s="29" t="str" cm="1">
+        <f t="array" ref="N24">IFERROR(_xlfn.IFS($H24-$M24=2,'Data Validation'!$D$2,$H24-$M24=1,'Data Validation'!$D$3,$H24-$M24=0,'Data Validation'!$D$4,$H24-$M24=-1,'Data Validation'!$D$5,$H24-$M24=-2,'Data Validation'!$D$6)," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="O24" s="30"/>
       <c r="P24" s="63"/>
     </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="169"/>
-      <c r="B25" s="170"/>
-      <c r="C25" s="171"/>
-      <c r="D25" s="172"/>
-      <c r="E25" s="170"/>
-      <c r="F25" s="173"/>
-      <c r="G25" s="172"/>
-      <c r="H25" s="172"/>
-      <c r="I25" s="174"/>
-      <c r="J25" s="174"/>
-      <c r="K25" s="173"/>
-      <c r="L25" s="175" t="s">
+    <row r="25" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="61"/>
+      <c r="B25" s="25">
+        <f>('Self-Assessment'!B28)</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="26">
+        <f>('Self-Assessment'!C28)</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="27">
+        <f>('Self-Assessment'!D28)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="28">
+        <f>('Self-Assessment'!E28)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="159"/>
+      <c r="G25" s="62">
+        <f>('Self-Assessment'!G28)</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="62" t="str">
+        <f>IFERROR(VLOOKUP(G25,'Data Validation'!$B$2:$C$4,2)," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I25" s="62">
+        <f>('Self-Assessment'!H28)</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="62">
+        <f>('Self-Assessment'!I28)</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="41"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="29" t="str">
+        <f>IFERROR(VLOOKUP(L25,'Data Validation'!$B$2:$C$4,2)," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="N25" s="29" t="str" cm="1">
+        <f t="array" ref="N25">IFERROR(_xlfn.IFS($H25-$M25=2,'Data Validation'!$D$2,$H25-$M25=1,'Data Validation'!$D$3,$H25-$M25=0,'Data Validation'!$D$4,$H25-$M25=-1,'Data Validation'!$D$5,$H25-$M25=-2,'Data Validation'!$D$6)," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="O25" s="30"/>
+      <c r="P25" s="63"/>
+    </row>
+    <row r="26" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="61"/>
+      <c r="B26" s="25">
+        <f>('Self-Assessment'!B29)</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="26">
+        <f>('Self-Assessment'!C29)</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="27">
+        <f>('Self-Assessment'!D29)</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="28">
+        <f>('Self-Assessment'!E29)</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="159"/>
+      <c r="G26" s="62">
+        <f>('Self-Assessment'!G29)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="62" t="str">
+        <f>IFERROR(VLOOKUP(G26,'Data Validation'!$B$2:$C$4,2)," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I26" s="62">
+        <f>('Self-Assessment'!H29)</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="62">
+        <f>('Self-Assessment'!I29)</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="41"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="29" t="str">
+        <f>IFERROR(VLOOKUP(L26,'Data Validation'!$B$2:$C$4,2)," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="N26" s="29" t="str" cm="1">
+        <f t="array" ref="N26">IFERROR(_xlfn.IFS($H26-$M26=2,'Data Validation'!$D$2,$H26-$M26=1,'Data Validation'!$D$3,$H26-$M26=0,'Data Validation'!$D$4,$H26-$M26=-1,'Data Validation'!$D$5,$H26-$M26=-2,'Data Validation'!$D$6)," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="O26" s="30"/>
+      <c r="P26" s="63"/>
+    </row>
+    <row r="27" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="61"/>
+      <c r="B27" s="25">
+        <f>('Self-Assessment'!B30)</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="26">
+        <f>('Self-Assessment'!C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="27">
+        <f>('Self-Assessment'!D30)</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="28">
+        <f>('Self-Assessment'!E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="159"/>
+      <c r="G27" s="62">
+        <f>('Self-Assessment'!G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="62" t="str">
+        <f>IFERROR(VLOOKUP(G27,'Data Validation'!$B$2:$C$4,2)," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I27" s="62">
+        <f>('Self-Assessment'!H30)</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="62">
+        <f>('Self-Assessment'!I30)</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="41"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="29" t="str">
+        <f>IFERROR(VLOOKUP(L27,'Data Validation'!$B$2:$C$4,2)," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="N27" s="29" t="str" cm="1">
+        <f t="array" ref="N27">IFERROR(_xlfn.IFS($H27-$M27=2,'Data Validation'!$D$2,$H27-$M27=1,'Data Validation'!$D$3,$H27-$M27=0,'Data Validation'!$D$4,$H27-$M27=-1,'Data Validation'!$D$5,$H27-$M27=-2,'Data Validation'!$D$6)," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="O27" s="30"/>
+      <c r="P27" s="63"/>
+    </row>
+    <row r="28" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="61"/>
+      <c r="B28" s="25">
+        <f>('Self-Assessment'!B31)</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="26">
+        <f>('Self-Assessment'!C31)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="27">
+        <f>('Self-Assessment'!D31)</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="28">
+        <f>('Self-Assessment'!E31)</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="159"/>
+      <c r="G28" s="62">
+        <f>('Self-Assessment'!G31)</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="62" t="str">
+        <f>IFERROR(VLOOKUP(G28,'Data Validation'!$B$2:$C$4,2)," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I28" s="62">
+        <f>('Self-Assessment'!H31)</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="62">
+        <f>('Self-Assessment'!I31)</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="41"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="29" t="str">
+        <f>IFERROR(VLOOKUP(L28,'Data Validation'!$B$2:$C$4,2)," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="N28" s="29" t="str" cm="1">
+        <f t="array" ref="N28">IFERROR(_xlfn.IFS($H28-$M28=2,'Data Validation'!$D$2,$H28-$M28=1,'Data Validation'!$D$3,$H28-$M28=0,'Data Validation'!$D$4,$H28-$M28=-1,'Data Validation'!$D$5,$H28-$M28=-2,'Data Validation'!$D$6)," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="O28" s="30"/>
+      <c r="P28" s="63"/>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="36"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="65"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="65"/>
+      <c r="M29" s="65"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="47"/>
+      <c r="P29" s="63"/>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="169"/>
+      <c r="B30" s="170"/>
+      <c r="C30" s="171"/>
+      <c r="D30" s="172"/>
+      <c r="E30" s="170"/>
+      <c r="F30" s="173"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="174"/>
+      <c r="J30" s="174"/>
+      <c r="K30" s="173"/>
+      <c r="L30" s="175" t="s">
         <v>38</v>
       </c>
-      <c r="M25" s="172"/>
-      <c r="N25" s="174"/>
-      <c r="O25" s="174"/>
-      <c r="P25" s="173"/>
-    </row>
-    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="169"/>
-      <c r="B26" s="170"/>
-      <c r="C26" s="171"/>
-      <c r="D26" s="172"/>
-      <c r="E26" s="170"/>
-      <c r="F26" s="173"/>
-      <c r="G26" s="172"/>
-      <c r="H26" s="172"/>
-      <c r="I26" s="174"/>
-      <c r="J26" s="174"/>
-      <c r="K26" s="173"/>
-      <c r="L26" s="186" t="s">
+      <c r="M30" s="172"/>
+      <c r="N30" s="174"/>
+      <c r="O30" s="174"/>
+      <c r="P30" s="173"/>
+    </row>
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="169"/>
+      <c r="B31" s="170"/>
+      <c r="C31" s="171"/>
+      <c r="D31" s="172"/>
+      <c r="E31" s="170"/>
+      <c r="F31" s="173"/>
+      <c r="G31" s="172"/>
+      <c r="H31" s="172"/>
+      <c r="I31" s="174"/>
+      <c r="J31" s="174"/>
+      <c r="K31" s="173"/>
+      <c r="L31" s="186" t="s">
         <v>39</v>
       </c>
-      <c r="M26" s="187"/>
-      <c r="N26" s="187"/>
-      <c r="O26" s="188"/>
-      <c r="P26" s="173"/>
-    </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="169"/>
-      <c r="B27" s="170"/>
-      <c r="C27" s="171"/>
-      <c r="D27" s="172"/>
-      <c r="E27" s="170"/>
-      <c r="F27" s="173"/>
-      <c r="G27" s="172"/>
-      <c r="H27" s="172"/>
-      <c r="I27" s="174"/>
-      <c r="J27" s="174"/>
-      <c r="K27" s="173"/>
-      <c r="L27" s="189"/>
-      <c r="M27" s="190"/>
-      <c r="N27" s="190"/>
-      <c r="O27" s="191"/>
-      <c r="P27" s="173"/>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="169"/>
-      <c r="B28" s="170"/>
-      <c r="C28" s="171"/>
-      <c r="D28" s="172"/>
-      <c r="E28" s="170"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="172"/>
-      <c r="H28" s="172"/>
-      <c r="I28" s="174"/>
-      <c r="J28" s="174"/>
-      <c r="K28" s="173"/>
-      <c r="L28" s="189"/>
-      <c r="M28" s="190"/>
-      <c r="N28" s="190"/>
-      <c r="O28" s="191"/>
-      <c r="P28" s="173"/>
-    </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="169"/>
-      <c r="B29" s="170"/>
-      <c r="C29" s="171"/>
-      <c r="D29" s="172"/>
-      <c r="E29" s="170"/>
-      <c r="F29" s="173"/>
-      <c r="G29" s="172"/>
-      <c r="H29" s="172"/>
-      <c r="I29" s="174"/>
-      <c r="J29" s="174"/>
-      <c r="K29" s="173"/>
-      <c r="L29" s="192"/>
-      <c r="M29" s="193"/>
-      <c r="N29" s="193"/>
-      <c r="O29" s="194"/>
-      <c r="P29" s="173"/>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="36"/>
-      <c r="B30" s="61"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="61"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="63"/>
-      <c r="L30" s="65"/>
-      <c r="M30" s="65"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="47"/>
-      <c r="P30" s="63"/>
-    </row>
-    <row r="31" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="61"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="156" t="s">
-        <v>40</v>
-      </c>
-      <c r="H31" s="66" t="str">
-        <f>IFERROR(ROUNDUP(AVERAGE($H$14:$H$23),2)," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="63"/>
-      <c r="L31" s="156" t="s">
-        <v>41</v>
-      </c>
-      <c r="M31" s="67" t="str">
-        <f>IFERROR(ROUNDUP(AVERAGE($M$14:$M$23),2)," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N31" s="47"/>
-      <c r="O31" s="47"/>
-      <c r="P31" s="63"/>
-    </row>
-    <row r="32" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="36"/>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="156" t="s">
-        <v>42</v>
-      </c>
-      <c r="H32" s="66" t="str">
-        <f>'Proficiency Calculations'!E16</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="63"/>
-      <c r="L32" s="156" t="s">
-        <v>43</v>
-      </c>
-      <c r="M32" s="67" t="str">
-        <f>'Proficiency Calculations'!E18</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N32" s="47"/>
-      <c r="O32" s="47"/>
-      <c r="P32" s="63"/>
-    </row>
-    <row r="33" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="36"/>
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="156" t="s">
-        <v>44</v>
-      </c>
-      <c r="H33" s="66" t="str">
-        <f>'Proficiency Calculations'!H16</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="63"/>
-      <c r="L33" s="156" t="s">
-        <v>45</v>
-      </c>
-      <c r="M33" s="67" t="str">
-        <f>'Proficiency Calculations'!H18</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N33" s="47"/>
-      <c r="O33" s="47"/>
-      <c r="P33" s="63"/>
-    </row>
-    <row r="34" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="36"/>
-      <c r="B34" s="61"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="156" t="s">
-        <v>46</v>
-      </c>
-      <c r="H34" s="66" t="str">
-        <f>'Proficiency Calculations'!I16</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="63"/>
-      <c r="L34" s="156" t="s">
-        <v>47</v>
-      </c>
-      <c r="M34" s="67" t="str">
-        <f>'Proficiency Calculations'!I18</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N34" s="47"/>
-      <c r="O34" s="47"/>
-      <c r="P34" s="65"/>
-    </row>
-    <row r="35" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M31" s="187"/>
+      <c r="N31" s="187"/>
+      <c r="O31" s="188"/>
+      <c r="P31" s="173"/>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="169"/>
+      <c r="B32" s="170"/>
+      <c r="C32" s="171"/>
+      <c r="D32" s="172"/>
+      <c r="E32" s="170"/>
+      <c r="F32" s="173"/>
+      <c r="G32" s="172"/>
+      <c r="H32" s="172"/>
+      <c r="I32" s="174"/>
+      <c r="J32" s="174"/>
+      <c r="K32" s="173"/>
+      <c r="L32" s="189"/>
+      <c r="M32" s="190"/>
+      <c r="N32" s="190"/>
+      <c r="O32" s="191"/>
+      <c r="P32" s="173"/>
+    </row>
+    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="169"/>
+      <c r="B33" s="170"/>
+      <c r="C33" s="171"/>
+      <c r="D33" s="172"/>
+      <c r="E33" s="170"/>
+      <c r="F33" s="173"/>
+      <c r="G33" s="172"/>
+      <c r="H33" s="172"/>
+      <c r="I33" s="174"/>
+      <c r="J33" s="174"/>
+      <c r="K33" s="173"/>
+      <c r="L33" s="189"/>
+      <c r="M33" s="190"/>
+      <c r="N33" s="190"/>
+      <c r="O33" s="191"/>
+      <c r="P33" s="173"/>
+    </row>
+    <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="169"/>
+      <c r="B34" s="170"/>
+      <c r="C34" s="171"/>
+      <c r="D34" s="172"/>
+      <c r="E34" s="170"/>
+      <c r="F34" s="173"/>
+      <c r="G34" s="172"/>
+      <c r="H34" s="172"/>
+      <c r="I34" s="174"/>
+      <c r="J34" s="174"/>
+      <c r="K34" s="173"/>
+      <c r="L34" s="192"/>
+      <c r="M34" s="193"/>
+      <c r="N34" s="193"/>
+      <c r="O34" s="194"/>
+      <c r="P34" s="173"/>
+    </row>
+    <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="36"/>
       <c r="B35" s="61"/>
       <c r="C35" s="64"/>
       <c r="D35" s="65"/>
       <c r="E35" s="61"/>
       <c r="F35" s="63"/>
-      <c r="G35" s="68" t="s">
-        <v>48</v>
-      </c>
-      <c r="H35" s="69" t="str">
-        <f>'Proficiency Calculations'!J16</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
       <c r="I35" s="47"/>
       <c r="J35" s="47"/>
       <c r="K35" s="63"/>
-      <c r="L35" s="68" t="s">
-        <v>49</v>
-      </c>
-      <c r="M35" s="70" t="str">
-        <f>'Proficiency Calculations'!J18</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="L35" s="65"/>
+      <c r="M35" s="65"/>
       <c r="N35" s="47"/>
-      <c r="O35" s="65"/>
-      <c r="P35" s="65"/>
+      <c r="O35" s="47"/>
+      <c r="P35" s="63"/>
     </row>
     <row r="36" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="36"/>
+      <c r="A36" s="61"/>
       <c r="B36" s="61"/>
-      <c r="C36" s="64"/>
+      <c r="C36" s="61"/>
       <c r="D36" s="65"/>
       <c r="E36" s="61"/>
       <c r="F36" s="63"/>
-      <c r="G36" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="H36" s="69" t="str">
-        <f>'Proficiency Calculations'!L16</f>
+      <c r="G36" s="156" t="s">
+        <v>40</v>
+      </c>
+      <c r="H36" s="66" t="str">
+        <f>IFERROR(ROUNDUP(AVERAGE($H$14:$H$28),2)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I36" s="47"/>
       <c r="J36" s="47"/>
       <c r="K36" s="63"/>
-      <c r="L36" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="M36" s="70" t="str">
-        <f>'Proficiency Calculations'!L18</f>
+      <c r="L36" s="156" t="s">
+        <v>41</v>
+      </c>
+      <c r="M36" s="67" t="str">
+        <f>IFERROR(ROUNDUP(AVERAGE($M$14:$M$28),2)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="N36" s="65"/>
-      <c r="O36" s="65"/>
-      <c r="P36" s="65"/>
+      <c r="N36" s="47"/>
+      <c r="O36" s="47"/>
+      <c r="P36" s="63"/>
     </row>
     <row r="37" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="36"/>
       <c r="B37" s="61"/>
-      <c r="C37" s="64"/>
+      <c r="C37" s="61"/>
       <c r="D37" s="65"/>
       <c r="E37" s="61"/>
       <c r="F37" s="63"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="65"/>
+      <c r="G37" s="156" t="s">
+        <v>42</v>
+      </c>
+      <c r="H37" s="66" t="str">
+        <f>'Proficiency Calculations'!E16</f>
+        <v xml:space="preserve"> </v>
+      </c>
       <c r="I37" s="47"/>
       <c r="J37" s="47"/>
       <c r="K37" s="63"/>
-      <c r="L37" s="68" t="s">
-        <v>51</v>
-      </c>
-      <c r="M37" s="71" t="str">
-        <f>'Proficiency Calculations'!D20</f>
+      <c r="L37" s="156" t="s">
+        <v>43</v>
+      </c>
+      <c r="M37" s="67" t="str">
+        <f>'Proficiency Calculations'!E18</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="N37" s="65"/>
-      <c r="O37" s="65"/>
-      <c r="P37" s="65"/>
+      <c r="N37" s="47"/>
+      <c r="O37" s="47"/>
+      <c r="P37" s="63"/>
     </row>
     <row r="38" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="36"/>
       <c r="B38" s="61"/>
-      <c r="C38" s="64"/>
+      <c r="C38" s="61"/>
       <c r="D38" s="65"/>
       <c r="E38" s="61"/>
       <c r="F38" s="63"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="65"/>
+      <c r="G38" s="156" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" s="66" t="str">
+        <f>'Proficiency Calculations'!H16</f>
+        <v xml:space="preserve"> </v>
+      </c>
       <c r="I38" s="47"/>
       <c r="J38" s="47"/>
       <c r="K38" s="63"/>
-      <c r="L38" s="65"/>
-      <c r="M38" s="65"/>
-      <c r="N38" s="65"/>
-      <c r="O38" s="65"/>
-      <c r="P38" s="65"/>
+      <c r="L38" s="156" t="s">
+        <v>45</v>
+      </c>
+      <c r="M38" s="67" t="str">
+        <f>'Proficiency Calculations'!H18</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="N38" s="47"/>
+      <c r="O38" s="47"/>
+      <c r="P38" s="63"/>
+    </row>
+    <row r="39" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="36"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="156" t="s">
+        <v>46</v>
+      </c>
+      <c r="H39" s="66" t="str">
+        <f>'Proficiency Calculations'!I16</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I39" s="47"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="63"/>
+      <c r="L39" s="156" t="s">
+        <v>47</v>
+      </c>
+      <c r="M39" s="67" t="str">
+        <f>'Proficiency Calculations'!I18</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="N39" s="47"/>
+      <c r="O39" s="47"/>
+      <c r="P39" s="65"/>
+    </row>
+    <row r="40" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="36"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="63"/>
+      <c r="G40" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="H40" s="69" t="str">
+        <f>'Proficiency Calculations'!J16</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I40" s="47"/>
+      <c r="J40" s="47"/>
+      <c r="K40" s="63"/>
+      <c r="L40" s="68" t="s">
+        <v>49</v>
+      </c>
+      <c r="M40" s="70" t="str">
+        <f>'Proficiency Calculations'!J18</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="N40" s="47"/>
+      <c r="O40" s="65"/>
+      <c r="P40" s="65"/>
+    </row>
+    <row r="41" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="36"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="H41" s="69" t="str">
+        <f>'Proficiency Calculations'!L16</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I41" s="47"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="63"/>
+      <c r="L41" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="M41" s="70" t="str">
+        <f>'Proficiency Calculations'!L18</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="N41" s="65"/>
+      <c r="O41" s="65"/>
+      <c r="P41" s="65"/>
+    </row>
+    <row r="42" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="36"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="63"/>
+      <c r="G42" s="65"/>
+      <c r="H42" s="65"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="63"/>
+      <c r="L42" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="M42" s="71" t="str">
+        <f>'Proficiency Calculations'!D20</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="N42" s="65"/>
+      <c r="O42" s="65"/>
+      <c r="P42" s="65"/>
+    </row>
+    <row r="43" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="36"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="64"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="63"/>
+      <c r="G43" s="65"/>
+      <c r="H43" s="65"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="63"/>
+      <c r="L43" s="65"/>
+      <c r="M43" s="65"/>
+      <c r="N43" s="65"/>
+      <c r="O43" s="65"/>
+      <c r="P43" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3510,9 +3780,9 @@
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="L12:O12"/>
-    <mergeCell ref="L26:O29"/>
+    <mergeCell ref="L31:O34"/>
   </mergeCells>
-  <conditionalFormatting sqref="H36 M36">
+  <conditionalFormatting sqref="H41 M41">
     <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>"Not marginal"</formula>
     </cfRule>
@@ -3520,7 +3790,7 @@
       <formula>"Marginal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M37">
+  <conditionalFormatting sqref="M42">
     <cfRule type="cellIs" dxfId="18" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -3528,7 +3798,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N14:N23">
+  <conditionalFormatting sqref="N14:N28">
     <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"2 below self-assessment"</formula>
     </cfRule>
@@ -3564,7 +3834,7 @@
           <x14:formula1>
             <xm:f>'Data Validation'!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>L14:L23</xm:sqref>
+          <xm:sqref>L14:L28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3984,7 +4254,7 @@
         <v>74</v>
       </c>
       <c r="C16" s="92" t="str">
-        <f>Evaluation!H31</f>
+        <f>Evaluation!H36</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D16" s="93"/>
@@ -4044,7 +4314,7 @@
       </c>
       <c r="C18" s="93"/>
       <c r="D18" s="97" t="str">
-        <f>(Evaluation!$M$31)</f>
+        <f>(Evaluation!$M$36)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E18" s="97" t="str">
@@ -4346,23 +4616,23 @@
         <v>0</v>
       </c>
       <c r="K2" s="167">
-        <f>'Self-Assessment'!$B$22</f>
+        <f>'Self-Assessment'!$B$27</f>
         <v>0</v>
       </c>
       <c r="L2" s="167">
-        <f>'Self-Assessment'!$B$23</f>
+        <f>'Self-Assessment'!$B$28</f>
         <v>0</v>
       </c>
       <c r="M2" s="167">
-        <f>'Self-Assessment'!$B$24</f>
+        <f>'Self-Assessment'!$B$29</f>
         <v>0</v>
       </c>
       <c r="N2" s="167">
-        <f>'Self-Assessment'!$B$25</f>
+        <f>'Self-Assessment'!$B$30</f>
         <v>0</v>
       </c>
       <c r="O2" s="167">
-        <f>'Self-Assessment'!$B$26</f>
+        <f>'Self-Assessment'!$B$31</f>
         <v>0</v>
       </c>
       <c r="P2" s="167" t="e">
@@ -4426,23 +4696,23 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="K3" s="103" t="str">
-        <f>Evaluation!$H$19</f>
+        <f>Evaluation!$H$24</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L3" s="103" t="str">
-        <f>Evaluation!$H$20</f>
+        <f>Evaluation!$H$25</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M3" s="103" t="str">
-        <f>Evaluation!$H$21</f>
+        <f>Evaluation!$H$26</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N3" s="103" t="str">
-        <f>Evaluation!$H$22</f>
+        <f>Evaluation!$H$27</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="O3" s="103" t="str">
-        <f>Evaluation!$H$23</f>
+        <f>Evaluation!$H$28</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P3" s="103" t="e">
@@ -4454,7 +4724,7 @@
         <v>#REF!</v>
       </c>
       <c r="R3" s="116" t="str">
-        <f>Evaluation!$H$31</f>
+        <f>Evaluation!$H$36</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4499,23 +4769,23 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="K4" s="103" t="str">
-        <f>Evaluation!$M$19</f>
+        <f>Evaluation!$M$24</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L4" s="103" t="str">
-        <f>Evaluation!$M$20</f>
+        <f>Evaluation!$M$25</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M4" s="103" t="str">
-        <f>Evaluation!$M$21</f>
+        <f>Evaluation!$M$26</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N4" s="103" t="str">
-        <f>Evaluation!$M$22</f>
+        <f>Evaluation!$M$27</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="O4" s="103" t="str">
-        <f>Evaluation!$M$23</f>
+        <f>Evaluation!$M$28</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P4" s="103" t="e">
@@ -4527,7 +4797,7 @@
         <v>#REF!</v>
       </c>
       <c r="R4" s="116" t="str">
-        <f>Evaluation!$M$31</f>
+        <f>Evaluation!$M$36</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -6140,24 +6410,24 @@
     <row r="19" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="25">
-        <f>('Self-Assessment'!B22)</f>
+        <f>('Self-Assessment'!B27)</f>
         <v>0</v>
       </c>
       <c r="C19" s="26">
-        <f>('Self-Assessment'!C22)</f>
+        <f>('Self-Assessment'!C27)</f>
         <v>0</v>
       </c>
       <c r="D19" s="27">
-        <f>('Self-Assessment'!D22)</f>
+        <f>('Self-Assessment'!D27)</f>
         <v>0</v>
       </c>
       <c r="E19" s="28">
-        <f>('Self-Assessment'!E22)</f>
+        <f>('Self-Assessment'!E27)</f>
         <v>0</v>
       </c>
       <c r="F19" s="159"/>
       <c r="G19" s="62">
-        <f>('Self-Assessment'!G22)</f>
+        <f>('Self-Assessment'!G27)</f>
         <v>0</v>
       </c>
       <c r="H19" s="62" t="str">
@@ -6165,28 +6435,28 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I19" s="62">
-        <f>('Self-Assessment'!H22)</f>
+        <f>('Self-Assessment'!H27)</f>
         <v>0</v>
       </c>
       <c r="J19" s="62">
-        <f>('Self-Assessment'!I22)</f>
+        <f>('Self-Assessment'!I27)</f>
         <v>0</v>
       </c>
       <c r="K19" s="63"/>
       <c r="L19" s="30">
-        <f>Evaluation!L19</f>
+        <f>Evaluation!L24</f>
         <v>0</v>
       </c>
       <c r="M19" s="29" t="str">
-        <f>Evaluation!M19</f>
+        <f>Evaluation!M24</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N19" s="29" t="str">
-        <f>Evaluation!N19</f>
+        <f>Evaluation!N24</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="O19" s="30">
-        <f>Evaluation!O19</f>
+        <f>Evaluation!O24</f>
         <v>0</v>
       </c>
       <c r="P19" s="63"/>
@@ -6194,24 +6464,24 @@
     <row r="20" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="61"/>
       <c r="B20" s="25">
-        <f>('Self-Assessment'!B23)</f>
+        <f>('Self-Assessment'!B28)</f>
         <v>0</v>
       </c>
       <c r="C20" s="26">
-        <f>('Self-Assessment'!C23)</f>
+        <f>('Self-Assessment'!C28)</f>
         <v>0</v>
       </c>
       <c r="D20" s="27">
-        <f>('Self-Assessment'!D23)</f>
+        <f>('Self-Assessment'!D28)</f>
         <v>0</v>
       </c>
       <c r="E20" s="28">
-        <f>('Self-Assessment'!E23)</f>
+        <f>('Self-Assessment'!E28)</f>
         <v>0</v>
       </c>
       <c r="F20" s="159"/>
       <c r="G20" s="62">
-        <f>('Self-Assessment'!G23)</f>
+        <f>('Self-Assessment'!G28)</f>
         <v>0</v>
       </c>
       <c r="H20" s="62" t="str">
@@ -6219,28 +6489,28 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I20" s="62">
-        <f>('Self-Assessment'!H23)</f>
+        <f>('Self-Assessment'!H28)</f>
         <v>0</v>
       </c>
       <c r="J20" s="62">
-        <f>('Self-Assessment'!I23)</f>
+        <f>('Self-Assessment'!I28)</f>
         <v>0</v>
       </c>
       <c r="K20" s="41"/>
       <c r="L20" s="30">
-        <f>Evaluation!L20</f>
+        <f>Evaluation!L25</f>
         <v>0</v>
       </c>
       <c r="M20" s="29" t="str">
-        <f>Evaluation!M20</f>
+        <f>Evaluation!M25</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N20" s="29" t="str">
-        <f>Evaluation!N20</f>
+        <f>Evaluation!N25</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="O20" s="30">
-        <f>Evaluation!O20</f>
+        <f>Evaluation!O25</f>
         <v>0</v>
       </c>
       <c r="P20" s="63"/>
@@ -6248,24 +6518,24 @@
     <row r="21" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="61"/>
       <c r="B21" s="25">
-        <f>('Self-Assessment'!B24)</f>
+        <f>('Self-Assessment'!B29)</f>
         <v>0</v>
       </c>
       <c r="C21" s="26">
-        <f>('Self-Assessment'!C24)</f>
+        <f>('Self-Assessment'!C29)</f>
         <v>0</v>
       </c>
       <c r="D21" s="27">
-        <f>('Self-Assessment'!D24)</f>
+        <f>('Self-Assessment'!D29)</f>
         <v>0</v>
       </c>
       <c r="E21" s="28">
-        <f>('Self-Assessment'!E24)</f>
+        <f>('Self-Assessment'!E29)</f>
         <v>0</v>
       </c>
       <c r="F21" s="159"/>
       <c r="G21" s="62">
-        <f>('Self-Assessment'!G24)</f>
+        <f>('Self-Assessment'!G29)</f>
         <v>0</v>
       </c>
       <c r="H21" s="62" t="str">
@@ -6273,28 +6543,28 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I21" s="62">
-        <f>('Self-Assessment'!H24)</f>
+        <f>('Self-Assessment'!H29)</f>
         <v>0</v>
       </c>
       <c r="J21" s="62">
-        <f>('Self-Assessment'!I24)</f>
+        <f>('Self-Assessment'!I29)</f>
         <v>0</v>
       </c>
       <c r="K21" s="41"/>
       <c r="L21" s="30">
-        <f>Evaluation!L21</f>
+        <f>Evaluation!L26</f>
         <v>0</v>
       </c>
       <c r="M21" s="29" t="str">
-        <f>Evaluation!M21</f>
+        <f>Evaluation!M26</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N21" s="29" t="str">
-        <f>Evaluation!N21</f>
+        <f>Evaluation!N26</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="O21" s="30">
-        <f>Evaluation!O21</f>
+        <f>Evaluation!O26</f>
         <v>0</v>
       </c>
       <c r="P21" s="63"/>
@@ -6302,24 +6572,24 @@
     <row r="22" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="61"/>
       <c r="B22" s="25">
-        <f>('Self-Assessment'!B25)</f>
+        <f>('Self-Assessment'!B30)</f>
         <v>0</v>
       </c>
       <c r="C22" s="26">
-        <f>('Self-Assessment'!C25)</f>
+        <f>('Self-Assessment'!C30)</f>
         <v>0</v>
       </c>
       <c r="D22" s="27">
-        <f>('Self-Assessment'!D25)</f>
+        <f>('Self-Assessment'!D30)</f>
         <v>0</v>
       </c>
       <c r="E22" s="28">
-        <f>('Self-Assessment'!E25)</f>
+        <f>('Self-Assessment'!E30)</f>
         <v>0</v>
       </c>
       <c r="F22" s="159"/>
       <c r="G22" s="62">
-        <f>('Self-Assessment'!G25)</f>
+        <f>('Self-Assessment'!G30)</f>
         <v>0</v>
       </c>
       <c r="H22" s="62" t="str">
@@ -6327,28 +6597,28 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I22" s="62">
-        <f>('Self-Assessment'!H25)</f>
+        <f>('Self-Assessment'!H30)</f>
         <v>0</v>
       </c>
       <c r="J22" s="62">
-        <f>('Self-Assessment'!I25)</f>
+        <f>('Self-Assessment'!I30)</f>
         <v>0</v>
       </c>
       <c r="K22" s="41"/>
       <c r="L22" s="30">
-        <f>Evaluation!L22</f>
+        <f>Evaluation!L27</f>
         <v>0</v>
       </c>
       <c r="M22" s="29" t="str">
-        <f>Evaluation!M22</f>
+        <f>Evaluation!M27</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N22" s="29" t="str">
-        <f>Evaluation!N22</f>
+        <f>Evaluation!N27</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="O22" s="30">
-        <f>Evaluation!O22</f>
+        <f>Evaluation!O27</f>
         <v>0</v>
       </c>
       <c r="P22" s="63"/>
@@ -6356,24 +6626,24 @@
     <row r="23" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="61"/>
       <c r="B23" s="25">
-        <f>('Self-Assessment'!B26)</f>
+        <f>('Self-Assessment'!B31)</f>
         <v>0</v>
       </c>
       <c r="C23" s="26">
-        <f>('Self-Assessment'!C26)</f>
+        <f>('Self-Assessment'!C31)</f>
         <v>0</v>
       </c>
       <c r="D23" s="27">
-        <f>('Self-Assessment'!D26)</f>
+        <f>('Self-Assessment'!D31)</f>
         <v>0</v>
       </c>
       <c r="E23" s="28">
-        <f>('Self-Assessment'!E26)</f>
+        <f>('Self-Assessment'!E31)</f>
         <v>0</v>
       </c>
       <c r="F23" s="159"/>
       <c r="G23" s="62">
-        <f>('Self-Assessment'!G26)</f>
+        <f>('Self-Assessment'!G31)</f>
         <v>0</v>
       </c>
       <c r="H23" s="62" t="str">
@@ -6381,28 +6651,28 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I23" s="62">
-        <f>('Self-Assessment'!H26)</f>
+        <f>('Self-Assessment'!H31)</f>
         <v>0</v>
       </c>
       <c r="J23" s="62">
-        <f>('Self-Assessment'!I26)</f>
+        <f>('Self-Assessment'!I31)</f>
         <v>0</v>
       </c>
       <c r="K23" s="41"/>
       <c r="L23" s="30">
-        <f>Evaluation!L23</f>
+        <f>Evaluation!L28</f>
         <v>0</v>
       </c>
       <c r="M23" s="29" t="str">
-        <f>Evaluation!M23</f>
+        <f>Evaluation!M28</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N23" s="29" t="str">
-        <f>Evaluation!N23</f>
+        <f>Evaluation!N28</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="O23" s="30">
-        <f>Evaluation!O23</f>
+        <f>Evaluation!O28</f>
         <v>0</v>
       </c>
       <c r="P23" s="63"/>
@@ -8435,7 +8705,7 @@
         <v>104</v>
       </c>
       <c r="C16" s="134" t="str">
-        <f>Evaluation!H31</f>
+        <f>Evaluation!H36</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D16" s="132"/>
@@ -8554,7 +8824,7 @@
         <v>106</v>
       </c>
       <c r="C20" s="140" t="str">
-        <f>Evaluation!M31</f>
+        <f>Evaluation!M36</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D20" s="127"/>

</xml_diff>